<commit_message>
Added padding for empty cell
</commit_message>
<xml_diff>
--- a/spec/fixtures/sample.xlsx
+++ b/spec/fixtures/sample.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t xml:space="preserve">First Name</t>
   </si>
@@ -35,6 +35,9 @@
     <t xml:space="preserve">Address</t>
   </si>
   <si>
+    <t xml:space="preserve">Surprise</t>
+  </si>
+  <si>
     <t xml:space="preserve">Phone</t>
   </si>
   <si>
@@ -59,6 +62,9 @@
     <t xml:space="preserve">0601020304</t>
   </si>
   <si>
+    <t xml:space="preserve">dsdsqd</t>
+  </si>
+  <si>
     <t xml:space="preserve">John</t>
   </si>
   <si>
@@ -72,6 +78,9 @@
   </si>
   <si>
     <t xml:space="preserve">123-456-7890</t>
+  </si>
+  <si>
+    <t xml:space="preserve">qdqsdq</t>
   </si>
   <si>
     <t xml:space="preserve">Not empty…</t>
@@ -191,20 +200,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I5" activeCellId="0" sqref="I5"/>
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="11.76"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -223,57 +231,76 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="0" t="n">
-        <v>10</v>
+      <c r="I2" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="0" t="n">
-        <v>12</v>
+      <c r="I4" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" display="john.smith@mail.com"/>
-    <hyperlink ref="C3" r:id="rId2" display="jean.lefebvre@mail.com"/>
+    <hyperlink ref="C4" r:id="rId2" display="jean.lefebvre@mail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -296,14 +323,11 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.64"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix issue with unknown cell type
</commit_message>
<xml_diff>
--- a/spec/fixtures/sample.xlsx
+++ b/spec/fixtures/sample.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t xml:space="preserve">First Name</t>
   </si>
@@ -44,6 +44,12 @@
     <t xml:space="preserve">Column with int</t>
   </si>
   <si>
+    <t xml:space="preserve">Column with float</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Column with str</t>
+  </si>
+  <si>
     <t xml:space="preserve">Empty column</t>
   </si>
   <si>
@@ -53,7 +59,7 @@
     <t xml:space="preserve">Lefebvre</t>
   </si>
   <si>
-    <t xml:space="preserve">john.smith@mail.com</t>
+    <t xml:space="preserve">john.lefebvre@mail.com</t>
   </si>
   <si>
     <t xml:space="preserve">75017 Paris</t>
@@ -62,6 +68,9 @@
     <t xml:space="preserve">0601020304</t>
   </si>
   <si>
+    <t xml:space="preserve">5073.01</t>
+  </si>
+  <si>
     <t xml:space="preserve">dsdsqd</t>
   </si>
   <si>
@@ -71,13 +80,16 @@
     <t xml:space="preserve">Smith</t>
   </si>
   <si>
-    <t xml:space="preserve">jean.lefebvre@mail.com</t>
+    <t xml:space="preserve">jean.smith@mail.com</t>
   </si>
   <si>
     <t xml:space="preserve">10013 New York</t>
   </si>
   <si>
     <t xml:space="preserve">123-456-7890</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0001.01</t>
   </si>
   <si>
     <t xml:space="preserve">qdqsdq</t>
@@ -94,7 +106,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Droid Sans"/>
@@ -115,6 +127,11 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Droid Sans"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -122,6 +139,12 @@
       <name val="Droid Sans"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -166,7 +189,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -179,7 +202,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -196,23 +227,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+      <selection pane="topLeft" activeCell="I5" activeCellId="0" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="11.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="7.41"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -237,74 +274,94 @@
       <c r="G1" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I1" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E2" s="1"/>
-      <c r="F2" s="3" t="s">
-        <v>12</v>
+      <c r="F2" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="G2" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="I2" s="0" t="s">
-        <v>13</v>
+      <c r="H2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="0" t="str">
+        <f aca="false">LEFT(H2,10)</f>
+        <v>5073.01</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
-      <c r="C3" s="2"/>
+      <c r="C3" s="3"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
-      <c r="F3" s="3"/>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F3" s="4"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="G4" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="I4" s="0" t="s">
-        <v>19</v>
+      <c r="H4" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" s="0" t="str">
+        <f aca="false">LEFT(H4,10)</f>
+        <v>0001.01</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="john.smith@mail.com"/>
-    <hyperlink ref="C4" r:id="rId2" display="jean.lefebvre@mail.com"/>
+    <hyperlink ref="C2" r:id="rId1" display="john.lefebvre@mail.com"/>
+    <hyperlink ref="C4" r:id="rId2" display="jean.smith@mail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Droid Serif,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Droid Serif,Regular"&amp;12Page &amp;P</oddFooter>
@@ -313,7 +370,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -323,17 +380,17 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Nimbus Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Nimbus Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>